<commit_message>
Módulo III - Sesión 1
</commit_message>
<xml_diff>
--- a/M209.xlsx
+++ b/M209.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Desktop/banjercito/banjercito-diplomado-datascience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Desktop/banjercito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA96FDA-D6ED-7A40-B43C-EAF5B97DB7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6EF195-64C5-D344-8053-57E5B198E7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31500" yWindow="-5640" windowWidth="29840" windowHeight="17820" xr2:uid="{B2A6D8AF-B744-844C-A2C8-985A7D99B8F5}"/>
+    <workbookView xWindow="-23460" yWindow="-5120" windowWidth="29840" windowHeight="17820" xr2:uid="{B2A6D8AF-B744-844C-A2C8-985A7D99B8F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>H + R</t>
+  </si>
+  <si>
+    <t>H + C</t>
+  </si>
+  <si>
+    <t>M+P</t>
+  </si>
+  <si>
+    <t>P+L</t>
+  </si>
+  <si>
+    <t>H+O</t>
   </si>
 </sst>
 </file>
@@ -488,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE406DF3-DD9A-8248-B073-F4449BB9EA6B}">
-  <dimension ref="D4:U59"/>
+  <dimension ref="D4:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D35"/>
+    <sheetView tabSelected="1" topLeftCell="F31" zoomScale="173" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,7 +516,7 @@
     <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:27" x14ac:dyDescent="0.2">
       <c r="J4" t="s">
         <v>1</v>
       </c>
@@ -515,7 +530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -567,8 +582,23 @@
       <c r="U5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D6" s="3">
         <v>1</v>
       </c>
@@ -585,19 +615,75 @@
         <v>16</v>
       </c>
       <c r="J6">
-        <f>IF($E6=$J$5,1,0)</f>
+        <f>IF($E6=J$5,1,0)</f>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>IF($E6=$K$5,1,0)</f>
+        <f t="shared" ref="K6:L21" si="0">IF($E6=K$5,1,0)</f>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>IF($E6=$L$5,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:21" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>IF($F6=M$5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f>IF($F6=N$5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>IF($F6=O$5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f>IF($G6=P$5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:R21" si="1">IF($G6=Q$5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f>IF($H6=S$5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6:U21" si="2">IF($H6=T$5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>J6*N6</f>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f>J6*T6</f>
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <f>K6*R6</f>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f>R6*S6</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <f>J6*M6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D7" s="3">
         <v>2</v>
       </c>
@@ -614,19 +700,75 @@
         <v>9</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:L35" si="0">IF($E7=$J$5,1,0)</f>
+        <f t="shared" ref="J7:L35" si="3">IF($E7=J$5,1,0)</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K35" si="1">IF($E7=$K$5,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L35" si="2">IF($E7=$L$5,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:21" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:O35" si="4">IF($F7=M$5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:R35" si="5">IF($G7=P$5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7:U35" si="6">IF($H7=S$5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f t="shared" ref="W7:W35" si="7">J7*N7</f>
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ref="X7:X35" si="8">J7*T7</f>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ref="Y7:Y35" si="9">K7*R7</f>
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ref="Z7:Z35" si="10">R7*S7</f>
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" ref="AA7:AA35" si="11">J7*M7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D8" s="3">
         <v>3</v>
       </c>
@@ -643,19 +785,75 @@
         <v>15</v>
       </c>
       <c r="J8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L8">
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D9" s="3">
         <v>4</v>
       </c>
@@ -672,19 +870,75 @@
         <v>9</v>
       </c>
       <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="U9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D10" s="3">
         <v>5</v>
       </c>
@@ -701,19 +955,75 @@
         <v>15</v>
       </c>
       <c r="J10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D11" s="3">
         <v>6</v>
       </c>
@@ -730,19 +1040,75 @@
         <v>16</v>
       </c>
       <c r="J11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D12" s="3">
         <v>7</v>
       </c>
@@ -759,19 +1125,75 @@
         <v>15</v>
       </c>
       <c r="J12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L12">
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D13" s="3">
         <v>8</v>
       </c>
@@ -788,19 +1210,75 @@
         <v>9</v>
       </c>
       <c r="J13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D14" s="3">
         <v>9</v>
       </c>
@@ -817,19 +1295,75 @@
         <v>15</v>
       </c>
       <c r="J14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L14">
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D15" s="3">
         <v>10</v>
       </c>
@@ -846,19 +1380,75 @@
         <v>16</v>
       </c>
       <c r="J15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15">
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D16" s="3">
         <v>11</v>
       </c>
@@ -875,19 +1465,75 @@
         <v>15</v>
       </c>
       <c r="J16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D17" s="3">
         <v>12</v>
       </c>
@@ -904,19 +1550,75 @@
         <v>15</v>
       </c>
       <c r="J17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D18" s="3">
         <v>13</v>
       </c>
@@ -933,19 +1635,75 @@
         <v>9</v>
       </c>
       <c r="J18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="U18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D19" s="3">
         <v>14</v>
       </c>
@@ -962,19 +1720,75 @@
         <v>16</v>
       </c>
       <c r="J19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q19">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D20" s="3">
         <v>15</v>
       </c>
@@ -991,19 +1805,75 @@
         <v>15</v>
       </c>
       <c r="J20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D21" s="3">
         <v>16</v>
       </c>
@@ -1020,19 +1890,75 @@
         <v>16</v>
       </c>
       <c r="J21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L21">
+      <c r="R21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D22" s="3">
         <v>17</v>
       </c>
@@ -1049,19 +1975,75 @@
         <v>9</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D23" s="3">
         <v>18</v>
       </c>
@@ -1078,19 +2060,75 @@
         <v>16</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D24" s="3">
         <v>19</v>
       </c>
@@ -1107,19 +2145,75 @@
         <v>15</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D25" s="3">
         <v>20</v>
       </c>
@@ -1136,19 +2230,75 @@
         <v>9</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D26" s="3">
         <v>21</v>
       </c>
@@ -1165,19 +2315,75 @@
         <v>16</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D27" s="3">
         <v>22</v>
       </c>
@@ -1194,19 +2400,75 @@
         <v>16</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D28" s="3">
         <v>23</v>
       </c>
@@ -1223,19 +2485,75 @@
         <v>15</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D29" s="3">
         <v>24</v>
       </c>
@@ -1252,19 +2570,75 @@
         <v>15</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D30" s="3">
         <v>25</v>
       </c>
@@ -1281,19 +2655,75 @@
         <v>16</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D31" s="3">
         <v>26</v>
       </c>
@@ -1310,19 +2740,75 @@
         <v>15</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D32" s="3">
         <v>27</v>
       </c>
@@ -1339,19 +2825,75 @@
         <v>15</v>
       </c>
       <c r="J32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D33" s="3">
         <v>28</v>
       </c>
@@ -1368,19 +2910,75 @@
         <v>15</v>
       </c>
       <c r="J33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D34" s="3">
         <v>29</v>
       </c>
@@ -1397,19 +2995,75 @@
         <v>9</v>
       </c>
       <c r="J34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D35" s="3">
         <v>30</v>
       </c>
@@ -1426,33 +3080,145 @@
         <v>16</v>
       </c>
       <c r="J35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L35">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:27" x14ac:dyDescent="0.2">
       <c r="J37">
         <f>SUM(J6:J35)</f>
         <v>9</v>
       </c>
       <c r="K37">
-        <f t="shared" ref="K37:L37" si="3">SUM(K6:K35)</f>
+        <f t="shared" ref="K37:M37" si="12">SUM(K6:K35)</f>
         <v>16</v>
       </c>
       <c r="L37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <f t="shared" si="12"/>
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ref="N37:W37" si="13">SUM(N6:N35)</f>
+        <v>10</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="X37">
+        <f>SUM(X6:X35)</f>
+        <v>3</v>
+      </c>
+      <c r="Y37">
+        <f>SUM(Y6:Y35)</f>
+        <v>5</v>
+      </c>
+      <c r="Z37">
+        <f>SUM(Z6:Z35)</f>
+        <v>4</v>
+      </c>
+      <c r="AA37">
+        <f>SUM(AA6:AA35)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="4:27" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
         <v>19</v>
       </c>
@@ -1465,28 +3231,133 @@
         <v>0.3</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" ref="K38:L38" si="4">AVERAGE(K6:K35)</f>
+        <f t="shared" ref="K38:M38" si="14">AVERAGE(K6:K35)</f>
         <v>0.53333333333333333</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M38" s="2">
+        <f t="shared" si="14"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" ref="N38:W38" si="15">AVERAGE(N6:N35)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.4</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="T38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2">
+        <f t="shared" si="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="X38" s="2">
+        <f t="shared" ref="X38:Y38" si="16">AVERAGE(X6:X35)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Y38" s="2">
+        <f t="shared" si="16"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="Z38" s="2">
+        <f t="shared" ref="Z38:AA38" si="17">AVERAGE(Z6:Z35)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="AA38" s="2">
+        <f t="shared" si="17"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="40" spans="4:27" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
         <v>17</v>
       </c>
       <c r="F40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
+        <v>2</v>
+      </c>
+      <c r="P40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>3</v>
+      </c>
+      <c r="K41" t="s">
+        <v>4</v>
+      </c>
+      <c r="L41" t="s">
+        <v>5</v>
+      </c>
+      <c r="M41" t="s">
+        <v>6</v>
+      </c>
+      <c r="N41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O41" t="s">
+        <v>8</v>
+      </c>
+      <c r="P41" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>10</v>
+      </c>
+      <c r="R41" t="s">
+        <v>11</v>
+      </c>
+      <c r="S41" t="s">
+        <v>9</v>
+      </c>
+      <c r="T41" t="s">
+        <v>16</v>
+      </c>
+      <c r="U41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +3371,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
         <v>4</v>
       </c>
@@ -1513,8 +3384,12 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <f>0.3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
         <v>5</v>
       </c>
@@ -1530,13 +3405,21 @@
         <f>SUM(F42:F44)</f>
         <v>0.99999999999999989</v>
       </c>
-    </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="45" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="46" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
         <v>6</v>
       </c>
@@ -1549,8 +3432,12 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <f>J45/J44</f>
+        <v>0.32075471698113206</v>
+      </c>
+    </row>
+    <row r="48" spans="4:27" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
         <v>7</v>
       </c>
@@ -1563,6 +3450,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G48" s="2"/>
+      <c r="J48">
+        <f>J45/J43</f>
+        <v>0.56666666666666676</v>
+      </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
@@ -1683,5 +3574,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>